<commit_message>
Documented results with OTSU preprocessing technique.
</commit_message>
<xml_diff>
--- a/Preprocessing Results/Preprocessing Results.xlsx
+++ b/Preprocessing Results/Preprocessing Results.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="45">
   <si>
     <t>Model</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>OTSU</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>OmO</t>
   </si>
 </sst>
 </file>
@@ -527,52 +536,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK54"/>
+  <dimension ref="A1:AM54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.33203125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6" customWidth="1"/>
-    <col min="20" max="22" width="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" customWidth="1"/>
+    <col min="13" max="13" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="0.77734375" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="22" max="24" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>31</v>
       </c>
@@ -598,91 +609,97 @@
         <v>40</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -711,86 +728,92 @@
         <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="3">
+      <c r="T2" s="1"/>
+      <c r="U2" s="3">
         <v>80.5</v>
       </c>
-      <c r="T2" s="1">
+      <c r="V2" s="1">
         <v>55.3</v>
       </c>
-      <c r="U2" s="1">
+      <c r="W2" s="1">
         <v>55.2</v>
       </c>
-      <c r="V2" s="1">
+      <c r="X2" s="1">
         <v>55.1</v>
       </c>
-      <c r="W2" s="1">
+      <c r="Y2" s="1">
         <v>89</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Z2" s="1">
         <v>82</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AA2" s="1">
         <v>74</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AB2" s="1">
         <v>89</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AC2" s="1">
         <v>72</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AD2" s="1">
         <v>87</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AE2" s="1">
         <v>78</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AF2" s="1">
         <v>89</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AG2" s="1">
         <v>80</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AH2" s="1">
         <v>70</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AI2" s="1">
         <v>76</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AJ2" s="1">
         <v>88</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AK2" s="1">
         <v>80</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AL2" s="1">
         <v>76</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AM2" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
@@ -814,11 +837,11 @@
         <v>41</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="L3" s="1" t="s">
         <v>41</v>
       </c>
@@ -832,71 +855,77 @@
         <v>41</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="3">
+      <c r="T3" s="1"/>
+      <c r="U3" s="3">
         <v>80.98</v>
       </c>
-      <c r="T3" s="1">
+      <c r="V3" s="1">
         <v>87.94</v>
       </c>
-      <c r="U3" s="1">
+      <c r="W3" s="1">
         <v>31.64</v>
       </c>
-      <c r="V3" s="1">
+      <c r="X3" s="1">
         <v>19.3</v>
       </c>
-      <c r="W3" s="1">
+      <c r="Y3" s="1">
         <v>70</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Z3" s="1">
         <v>78</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="AA3" s="1">
         <v>76</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AB3" s="1">
         <v>90</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AC3" s="1">
         <v>71</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AD3" s="1">
         <v>87</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AE3" s="1">
         <v>77</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AF3" s="1">
         <v>77</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AG3" s="1">
         <v>88</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AH3" s="1">
         <v>89</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AI3" s="1">
         <v>81</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AJ3" s="1">
         <v>88</v>
       </c>
-      <c r="AI3" s="1">
+      <c r="AK3" s="1">
         <v>74</v>
       </c>
-      <c r="AJ3" s="1">
+      <c r="AL3" s="1">
         <v>80</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AM3" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
@@ -925,86 +954,92 @@
         <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="3">
+      <c r="T4" s="1"/>
+      <c r="U4" s="3">
         <v>80.3</v>
       </c>
-      <c r="T4" s="1">
+      <c r="V4" s="1">
         <v>56.3</v>
       </c>
-      <c r="U4" s="1">
+      <c r="W4" s="1">
         <v>55</v>
       </c>
-      <c r="V4" s="1">
+      <c r="X4" s="1">
         <v>53.6</v>
       </c>
-      <c r="W4" s="1">
+      <c r="Y4" s="1">
         <v>87</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Z4" s="1">
         <v>72</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AA4" s="1">
         <v>76</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AB4" s="1">
         <v>69</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AC4" s="1">
         <v>89</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AD4" s="1">
         <v>78</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AE4" s="1">
         <v>78</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AF4" s="1">
         <v>80</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AG4" s="1">
         <v>87</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AH4" s="1">
         <v>87</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AI4" s="1">
         <v>72</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AJ4" s="1">
         <v>89</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AK4" s="1">
         <v>79</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AL4" s="1">
         <v>79</v>
       </c>
-      <c r="AK4" s="1">
+      <c r="AM4" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
@@ -1028,11 +1063,11 @@
         <v>41</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="L5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1046,71 +1081,77 @@
         <v>41</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="3">
+      <c r="T5" s="1"/>
+      <c r="U5" s="3">
         <v>80.8</v>
       </c>
-      <c r="T5" s="1">
+      <c r="V5" s="1">
         <v>93.8</v>
       </c>
-      <c r="U5" s="1">
+      <c r="W5" s="1">
         <v>26.8</v>
       </c>
-      <c r="V5" s="1">
+      <c r="X5" s="1">
         <v>15.6</v>
       </c>
-      <c r="W5" s="1">
+      <c r="Y5" s="1">
         <v>77</v>
       </c>
-      <c r="X5" s="1">
+      <c r="Z5" s="1">
         <v>69</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>80</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>78</v>
       </c>
       <c r="AA5" s="1">
         <v>80</v>
       </c>
       <c r="AB5" s="1">
+        <v>78</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>80</v>
+      </c>
+      <c r="AD5" s="1">
         <v>86</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AE5" s="1">
         <v>89</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="AF5" s="1">
         <v>66</v>
       </c>
-      <c r="AE5" s="1">
+      <c r="AG5" s="1">
         <v>90</v>
       </c>
-      <c r="AF5" s="1">
+      <c r="AH5" s="1">
         <v>80</v>
       </c>
-      <c r="AG5" s="1">
+      <c r="AI5" s="1">
         <v>83</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AJ5" s="1">
         <v>89</v>
       </c>
-      <c r="AI5" s="1">
+      <c r="AK5" s="1">
         <v>87</v>
       </c>
-      <c r="AJ5" s="1">
+      <c r="AL5" s="1">
         <v>74</v>
       </c>
-      <c r="AK5" s="1">
+      <c r="AM5" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>5</v>
       </c>
@@ -1137,86 +1178,92 @@
         <v>41</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="N6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="3">
+      <c r="T6" s="1"/>
+      <c r="U6" s="3">
         <v>78</v>
       </c>
-      <c r="T6" s="1">
+      <c r="V6" s="1">
         <v>51.4</v>
       </c>
-      <c r="U6" s="1">
+      <c r="W6" s="1">
         <v>53.2</v>
       </c>
-      <c r="V6" s="1">
+      <c r="X6" s="1">
         <v>55.2</v>
       </c>
-      <c r="W6" s="1">
+      <c r="Y6" s="1">
         <v>72</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Z6" s="1">
         <v>76</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AA6" s="1">
         <v>78</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AB6" s="1">
         <v>88</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AC6" s="1">
         <v>69</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AD6" s="1">
         <v>79</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AE6" s="1">
         <v>86</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AF6" s="1">
         <v>72</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AG6" s="1">
         <v>78</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AH6" s="1">
         <v>73</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AI6" s="1">
         <v>75</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AJ6" s="1">
         <v>84</v>
       </c>
-      <c r="AI6" s="1">
+      <c r="AK6" s="1">
         <v>84</v>
       </c>
-      <c r="AJ6" s="1">
+      <c r="AL6" s="1">
         <v>85</v>
       </c>
-      <c r="AK6" s="1">
+      <c r="AM6" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
@@ -1240,89 +1287,95 @@
         <v>41</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="L7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="3">
+      <c r="T7" s="1"/>
+      <c r="U7" s="3">
         <v>80</v>
       </c>
-      <c r="T7" s="1">
+      <c r="V7" s="1">
         <v>56.3</v>
       </c>
-      <c r="U7" s="1">
+      <c r="W7" s="1">
         <v>54.4</v>
       </c>
-      <c r="V7" s="1">
+      <c r="X7" s="1">
         <v>52.5</v>
       </c>
-      <c r="W7" s="1">
+      <c r="Y7" s="1">
         <v>77</v>
       </c>
-      <c r="X7" s="1">
+      <c r="Z7" s="1">
         <v>90</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="AA7" s="1">
         <v>88</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="AB7" s="1">
         <v>87</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AC7" s="1">
         <v>83</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AD7" s="1">
         <v>72</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AE7" s="1">
         <v>69</v>
       </c>
-      <c r="AD7" s="1">
+      <c r="AF7" s="1">
         <v>80</v>
       </c>
-      <c r="AE7" s="1">
+      <c r="AG7" s="1">
         <v>87</v>
       </c>
-      <c r="AF7" s="1">
+      <c r="AH7" s="1">
         <v>75</v>
       </c>
-      <c r="AG7" s="1">
+      <c r="AI7" s="1">
         <v>79</v>
       </c>
-      <c r="AH7" s="1">
+      <c r="AJ7" s="1">
         <v>76</v>
       </c>
-      <c r="AI7" s="1">
+      <c r="AK7" s="1">
         <v>72</v>
       </c>
-      <c r="AJ7" s="1">
+      <c r="AL7" s="1">
         <v>84</v>
       </c>
-      <c r="AK7" s="1">
+      <c r="AM7" s="1">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>7</v>
       </c>
@@ -1342,98 +1395,101 @@
         <v>300</v>
       </c>
       <c r="H8" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="L8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="P8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="3">
+      <c r="T8" s="1"/>
+      <c r="U8" s="3">
         <v>80.599999999999994</v>
       </c>
-      <c r="T8" s="1">
+      <c r="V8" s="1">
         <v>93.4</v>
       </c>
-      <c r="U8" s="1">
+      <c r="W8" s="1">
         <v>26</v>
       </c>
-      <c r="V8" s="1">
+      <c r="X8" s="1">
         <v>15</v>
       </c>
-      <c r="W8" s="1">
+      <c r="Y8" s="1">
         <v>82</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Z8" s="1">
         <v>73</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AA8" s="1">
         <v>88</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AB8" s="1">
         <v>79</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AC8" s="1">
         <v>90</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AD8" s="1">
         <v>68</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AE8" s="1">
         <v>79</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AF8" s="1">
         <v>76</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AG8" s="1">
         <v>87</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AH8" s="1">
         <v>88</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AI8" s="1">
         <v>86</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AJ8" s="1">
         <v>76</v>
       </c>
-      <c r="AI8" s="1">
+      <c r="AK8" s="1">
         <v>90</v>
       </c>
-      <c r="AJ8" s="1">
+      <c r="AL8" s="1">
         <v>71</v>
       </c>
-      <c r="AK8" s="1">
+      <c r="AM8" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>8</v>
-      </c>
+    <row r="9" spans="2:39" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1469,131 +1525,352 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
-    </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+    </row>
+    <row r="10" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>224</v>
+      </c>
+      <c r="H10" s="1">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1">
+        <v>76.3</v>
+      </c>
+      <c r="V10" s="1">
+        <v>51</v>
+      </c>
+      <c r="W10" s="1">
+        <v>52</v>
+      </c>
+      <c r="X10" s="1">
+        <v>53</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>74</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>70</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>77</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>67</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>84</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>75</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>75</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>82</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>68</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>78</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>83</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>86</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>76</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>65</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>9</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-    </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B11">
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="F11" s="1">
         <v>10</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
+      <c r="G11" s="1">
+        <v>224</v>
+      </c>
+      <c r="H11" s="1">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-    </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="U11" s="1">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="V11" s="1">
+        <v>51.4</v>
+      </c>
+      <c r="W11" s="1">
+        <v>52.8</v>
+      </c>
+      <c r="X11" s="1">
+        <v>53.2</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>75</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>70</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>78</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>67</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>84</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>75</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>74</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>84</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>67</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>77</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>82</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>87</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>76</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>75</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>224</v>
+      </c>
+      <c r="H12" s="1">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-    </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>12</v>
-      </c>
+      <c r="U12" s="1">
+        <v>75.2</v>
+      </c>
+      <c r="V12" s="1">
+        <v>51.5</v>
+      </c>
+      <c r="W12" s="1">
+        <v>51.7</v>
+      </c>
+      <c r="X12" s="1">
+        <v>52</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>73</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>66</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>77</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>66</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>82</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>72</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>72</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>83</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>66</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>76</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>81</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>85</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>74</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>73</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="2:39" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1629,11 +1906,10 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
-    </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>13</v>
-      </c>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+    </row>
+    <row r="14" spans="2:39" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1669,8 +1945,10 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
-    </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+    </row>
+    <row r="15" spans="2:39" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1691,8 +1969,10 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="2:39" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1713,8 +1993,10 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1735,8 +2017,10 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1757,8 +2041,10 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1779,8 +2065,10 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1801,8 +2089,10 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1823,8 +2113,10 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1845,8 +2137,10 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1867,8 +2161,10 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1889,8 +2185,10 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1911,8 +2209,10 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1933,8 +2233,10 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1955,8 +2257,10 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1977,8 +2281,10 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1999,8 +2305,10 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -2021,8 +2329,10 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2043,8 +2353,10 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2065,8 +2377,10 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
-    </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2087,8 +2401,10 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
-    </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2109,8 +2425,10 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
-    </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -2131,8 +2449,10 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2153,8 +2473,10 @@
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -2175,8 +2497,10 @@
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2197,8 +2521,10 @@
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
-    </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -2219,8 +2545,10 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
-    </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2241,8 +2569,10 @@
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
-    </row>
-    <row r="41" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2263,8 +2593,10 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2285,8 +2617,10 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
-    </row>
-    <row r="43" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2307,8 +2641,10 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
-    </row>
-    <row r="44" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2329,8 +2665,10 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
-    </row>
-    <row r="45" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2351,8 +2689,10 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+    </row>
+    <row r="46" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2373,8 +2713,10 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+    </row>
+    <row r="47" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2395,8 +2737,10 @@
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2417,8 +2761,10 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2439,8 +2785,10 @@
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2461,8 +2809,10 @@
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
-    </row>
-    <row r="51" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2483,8 +2833,10 @@
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2505,8 +2857,10 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
-    </row>
-    <row r="53" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+    </row>
+    <row r="53" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2527,8 +2881,10 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+    </row>
+    <row r="54" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2549,6 +2905,8 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tried MobileNet on mutually exclusive samples.
</commit_message>
<xml_diff>
--- a/Preprocessing Results/Preprocessing Results.xlsx
+++ b/Preprocessing Results/Preprocessing Results.xlsx
@@ -224,12 +224,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,6 +262,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +552,7 @@
   <dimension ref="A1:AM54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,7 +713,7 @@
       </c>
     </row>
     <row r="2" spans="2:39" x14ac:dyDescent="0.3">
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -755,16 +768,16 @@
         <v>6</v>
       </c>
       <c r="T2" s="1"/>
-      <c r="U2" s="3">
+      <c r="U2" s="6">
         <v>80.5</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="7">
         <v>55.3</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="7">
         <v>55.2</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2" s="7">
         <v>55.1</v>
       </c>
       <c r="Y2" s="1">
@@ -926,7 +939,7 @@
       </c>
     </row>
     <row r="4" spans="2:39" x14ac:dyDescent="0.3">
-      <c r="B4">
+      <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -981,16 +994,16 @@
         <v>6</v>
       </c>
       <c r="T4" s="1"/>
-      <c r="U4" s="3">
+      <c r="U4" s="6">
         <v>80.3</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="7">
         <v>56.3</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="7">
         <v>55</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="7">
         <v>53.6</v>
       </c>
       <c r="Y4" s="1">

</xml_diff>